<commit_message>
Fix BATTERY STORAGE, U2 to be NCAP_FOM~2020
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
+++ b/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\times-ireland-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094C92C0-F1DC-48EC-BAE1-F5ADC5E21510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026C833B-FCFF-4DA3-9BD7-E2C11CF1BD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Specify techno-economic data for battery storage technologies</t>
+  </si>
+  <si>
+    <t>NCAP_FOM~2020</t>
   </si>
 </sst>
 </file>
@@ -1242,24 +1245,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.73046875" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" customWidth="1"/>
+    <col min="8" max="10" width="8.1328125" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.3984375" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1287,7 +1290,7 @@
       <c r="Y1" s="14"/>
       <c r="Z1" s="14"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1315,7 +1318,7 @@
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1343,7 +1346,7 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1371,7 +1374,7 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1399,7 +1402,7 @@
       <c r="Y5" s="14"/>
       <c r="Z5" s="14"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1427,7 +1430,7 @@
       <c r="Y6" s="14"/>
       <c r="Z6" s="14"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1455,7 +1458,7 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1483,7 +1486,7 @@
       <c r="Y8" s="14"/>
       <c r="Z8" s="14"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1511,7 +1514,7 @@
       <c r="Y9" s="14"/>
       <c r="Z9" s="14"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1539,7 +1542,7 @@
       <c r="Y10" s="14"/>
       <c r="Z10" s="14"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1567,7 +1570,7 @@
       <c r="Y11" s="14"/>
       <c r="Z11" s="14"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1595,7 +1598,7 @@
       <c r="Y12" s="14"/>
       <c r="Z12" s="14"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1623,7 +1626,7 @@
       <c r="Y13" s="14"/>
       <c r="Z13" s="14"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1651,7 +1654,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1679,7 +1682,7 @@
       <c r="Y15" s="14"/>
       <c r="Z15" s="14"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="29" t="s">
         <v>52</v>
       </c>
@@ -1709,7 +1712,7 @@
       <c r="Y16" s="14"/>
       <c r="Z16" s="14"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1737,7 +1740,7 @@
       <c r="Y17" s="14"/>
       <c r="Z17" s="14"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1765,7 +1768,7 @@
       <c r="Y18" s="14"/>
       <c r="Z18" s="14"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="20" t="s">
         <v>53</v>
       </c>
@@ -1797,7 +1800,7 @@
       <c r="Y19" s="14"/>
       <c r="Z19" s="14"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="20" t="s">
         <v>54</v>
       </c>
@@ -1829,7 +1832,7 @@
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="20" t="s">
         <v>55</v>
       </c>
@@ -1861,7 +1864,7 @@
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="20"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -1889,7 +1892,7 @@
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="20" t="s">
         <v>56</v>
       </c>
@@ -1921,7 +1924,7 @@
       <c r="Y23" s="14"/>
       <c r="Z23" s="14"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="20"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -1949,7 +1952,7 @@
       <c r="Y24" s="14"/>
       <c r="Z24" s="14"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="20"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -1977,7 +1980,7 @@
       <c r="Y25" s="14"/>
       <c r="Z25" s="14"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="20" t="s">
         <v>57</v>
       </c>
@@ -2009,7 +2012,7 @@
       <c r="Y26" s="14"/>
       <c r="Z26" s="14"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="20"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -2037,7 +2040,7 @@
       <c r="Y27" s="14"/>
       <c r="Z27" s="14"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="20"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -2065,7 +2068,7 @@
       <c r="Y28" s="14"/>
       <c r="Z28" s="14"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="20" t="s">
         <v>58</v>
       </c>
@@ -2097,7 +2100,7 @@
       <c r="Y29" s="14"/>
       <c r="Z29" s="14"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="20" t="s">
         <v>59</v>
       </c>
@@ -2129,7 +2132,7 @@
       <c r="Y30" s="14"/>
       <c r="Z30" s="14"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="20" t="s">
         <v>61</v>
       </c>
@@ -2161,7 +2164,7 @@
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="26"/>
       <c r="B32" s="27" t="s">
         <v>63</v>
@@ -2191,7 +2194,7 @@
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -2219,7 +2222,7 @@
       <c r="Y33" s="14"/>
       <c r="Z33" s="14"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -2247,7 +2250,7 @@
       <c r="Y34" s="14"/>
       <c r="Z34" s="14"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -2275,7 +2278,7 @@
       <c r="Y35" s="14"/>
       <c r="Z35" s="14"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2303,7 +2306,7 @@
       <c r="Y36" s="14"/>
       <c r="Z36" s="14"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -2331,7 +2334,7 @@
       <c r="Y37" s="14"/>
       <c r="Z37" s="14"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -2359,7 +2362,7 @@
       <c r="Y38" s="14"/>
       <c r="Z38" s="14"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -2387,7 +2390,7 @@
       <c r="Y39" s="14"/>
       <c r="Z39" s="14"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -2415,7 +2418,7 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="14"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -2443,7 +2446,7 @@
       <c r="Y41" s="14"/>
       <c r="Z41" s="14"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -2471,7 +2474,7 @@
       <c r="Y42" s="14"/>
       <c r="Z42" s="14"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -2499,7 +2502,7 @@
       <c r="Y43" s="14"/>
       <c r="Z43" s="14"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -2527,7 +2530,7 @@
       <c r="Y44" s="14"/>
       <c r="Z44" s="14"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -2555,7 +2558,7 @@
       <c r="Y45" s="14"/>
       <c r="Z45" s="14"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -2583,7 +2586,7 @@
       <c r="Y46" s="14"/>
       <c r="Z46" s="14"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -2611,7 +2614,7 @@
       <c r="Y47" s="14"/>
       <c r="Z47" s="14"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -2639,7 +2642,7 @@
       <c r="Y48" s="14"/>
       <c r="Z48" s="14"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -2667,7 +2670,7 @@
       <c r="Y49" s="14"/>
       <c r="Z49" s="14"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -2695,7 +2698,7 @@
       <c r="Y50" s="14"/>
       <c r="Z50" s="14"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -2723,7 +2726,7 @@
       <c r="Y51" s="14"/>
       <c r="Z51" s="14"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -2751,7 +2754,7 @@
       <c r="Y52" s="14"/>
       <c r="Z52" s="14"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -2779,7 +2782,7 @@
       <c r="Y53" s="14"/>
       <c r="Z53" s="14"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -2807,7 +2810,7 @@
       <c r="Y54" s="14"/>
       <c r="Z54" s="14"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -2835,7 +2838,7 @@
       <c r="Y55" s="14"/>
       <c r="Z55" s="14"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -2863,7 +2866,7 @@
       <c r="Y56" s="14"/>
       <c r="Z56" s="14"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -2891,7 +2894,7 @@
       <c r="Y57" s="14"/>
       <c r="Z57" s="14"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -2919,7 +2922,7 @@
       <c r="Y58" s="14"/>
       <c r="Z58" s="14"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
@@ -2947,7 +2950,7 @@
       <c r="Y59" s="14"/>
       <c r="Z59" s="14"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -2975,7 +2978,7 @@
       <c r="Y60" s="14"/>
       <c r="Z60" s="14"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
@@ -3003,7 +3006,7 @@
       <c r="Y61" s="14"/>
       <c r="Z61" s="14"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
@@ -3031,7 +3034,7 @@
       <c r="Y62" s="14"/>
       <c r="Z62" s="14"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -3059,7 +3062,7 @@
       <c r="Y63" s="14"/>
       <c r="Z63" s="14"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
@@ -3087,7 +3090,7 @@
       <c r="Y64" s="14"/>
       <c r="Z64" s="14"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
@@ -3115,7 +3118,7 @@
       <c r="Y65" s="14"/>
       <c r="Z65" s="14"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
@@ -3143,7 +3146,7 @@
       <c r="Y66" s="14"/>
       <c r="Z66" s="14"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
@@ -3171,7 +3174,7 @@
       <c r="Y67" s="14"/>
       <c r="Z67" s="14"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
@@ -3199,7 +3202,7 @@
       <c r="Y68" s="14"/>
       <c r="Z68" s="14"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
@@ -3227,7 +3230,7 @@
       <c r="Y69" s="14"/>
       <c r="Z69" s="14"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
@@ -3255,7 +3258,7 @@
       <c r="Y70" s="14"/>
       <c r="Z70" s="14"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
@@ -3283,7 +3286,7 @@
       <c r="Y71" s="14"/>
       <c r="Z71" s="14"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
@@ -3311,7 +3314,7 @@
       <c r="Y72" s="14"/>
       <c r="Z72" s="14"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -3339,7 +3342,7 @@
       <c r="Y73" s="14"/>
       <c r="Z73" s="14"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
@@ -3367,7 +3370,7 @@
       <c r="Y74" s="14"/>
       <c r="Z74" s="14"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -3395,7 +3398,7 @@
       <c r="Y75" s="14"/>
       <c r="Z75" s="14"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
@@ -3423,7 +3426,7 @@
       <c r="Y76" s="14"/>
       <c r="Z76" s="14"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
@@ -3451,7 +3454,7 @@
       <c r="Y77" s="14"/>
       <c r="Z77" s="14"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14"/>
@@ -3479,7 +3482,7 @@
       <c r="Y78" s="14"/>
       <c r="Z78" s="14"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
@@ -3507,7 +3510,7 @@
       <c r="Y79" s="14"/>
       <c r="Z79" s="14"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A80" s="14"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
@@ -3535,7 +3538,7 @@
       <c r="Y80" s="14"/>
       <c r="Z80" s="14"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A81" s="14"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
@@ -3563,7 +3566,7 @@
       <c r="Y81" s="14"/>
       <c r="Z81" s="14"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A82" s="14"/>
       <c r="B82" s="14"/>
       <c r="C82" s="14"/>
@@ -3591,7 +3594,7 @@
       <c r="Y82" s="14"/>
       <c r="Z82" s="14"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
@@ -3619,7 +3622,7 @@
       <c r="Y83" s="14"/>
       <c r="Z83" s="14"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
@@ -3647,7 +3650,7 @@
       <c r="Y84" s="14"/>
       <c r="Z84" s="14"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
@@ -3675,7 +3678,7 @@
       <c r="Y85" s="14"/>
       <c r="Z85" s="14"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -3703,7 +3706,7 @@
       <c r="Y86" s="14"/>
       <c r="Z86" s="14"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" s="14"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -3731,7 +3734,7 @@
       <c r="Y87" s="14"/>
       <c r="Z87" s="14"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" s="14"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -3759,7 +3762,7 @@
       <c r="Y88" s="14"/>
       <c r="Z88" s="14"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A89" s="14"/>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
@@ -3787,7 +3790,7 @@
       <c r="Y89" s="14"/>
       <c r="Z89" s="14"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A90" s="14"/>
       <c r="B90" s="14"/>
       <c r="C90" s="14"/>
@@ -3815,7 +3818,7 @@
       <c r="Y90" s="14"/>
       <c r="Z90" s="14"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A91" s="14"/>
       <c r="B91" s="14"/>
       <c r="C91" s="14"/>
@@ -3843,7 +3846,7 @@
       <c r="Y91" s="14"/>
       <c r="Z91" s="14"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A92" s="14"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
@@ -3871,7 +3874,7 @@
       <c r="Y92" s="14"/>
       <c r="Z92" s="14"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A93" s="14"/>
       <c r="B93" s="14"/>
       <c r="C93" s="14"/>
@@ -3899,7 +3902,7 @@
       <c r="Y93" s="14"/>
       <c r="Z93" s="14"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A94" s="14"/>
       <c r="B94" s="14"/>
       <c r="C94" s="14"/>
@@ -3927,7 +3930,7 @@
       <c r="Y94" s="14"/>
       <c r="Z94" s="14"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
@@ -3955,7 +3958,7 @@
       <c r="Y95" s="14"/>
       <c r="Z95" s="14"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -3983,7 +3986,7 @@
       <c r="Y96" s="14"/>
       <c r="Z96" s="14"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A97" s="14"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
@@ -4011,7 +4014,7 @@
       <c r="Y97" s="14"/>
       <c r="Z97" s="14"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
@@ -4039,7 +4042,7 @@
       <c r="Y98" s="14"/>
       <c r="Z98" s="14"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A99" s="14"/>
       <c r="B99" s="14"/>
       <c r="C99" s="14"/>
@@ -4094,30 +4097,30 @@
   </sheetPr>
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="43.7109375" customWidth="1"/>
-    <col min="12" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" customWidth="1"/>
-    <col min="20" max="23" width="12.42578125" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.3984375" customWidth="1"/>
+    <col min="11" max="11" width="43.73046875" customWidth="1"/>
+    <col min="12" max="13" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.3984375" customWidth="1"/>
+    <col min="19" max="19" width="10.86328125" customWidth="1"/>
+    <col min="20" max="23" width="12.3984375" customWidth="1"/>
+    <col min="24" max="24" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4146,7 +4149,7 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>2</v>
@@ -4203,7 +4206,7 @@
         <v>17</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="V2" s="6" t="s">
         <v>19</v>
@@ -4218,7 +4221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="101.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>22</v>
@@ -4274,7 +4277,7 @@
       </c>
       <c r="Y3" s="8"/>
     </row>
-    <row r="4" spans="1:27" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="43.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -4323,7 +4326,7 @@
       </c>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>41</v>
       </c>
@@ -4396,7 +4399,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
@@ -4466,7 +4469,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
@@ -4536,7 +4539,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -4545,7 +4548,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -4554,7 +4557,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>

</xml_diff>